<commit_message>
Update weekly tracker 17/08/2021
- Charts
- Data
</commit_message>
<xml_diff>
--- a/Data/quarterly_charts_q1.xlsx
+++ b/Data/quarterly_charts_q1.xlsx
@@ -28,103 +28,112 @@
     <t>ESP</t>
   </si>
   <si>
+    <t>PRT</t>
+  </si>
+  <si>
     <t>ISL</t>
   </si>
   <si>
-    <t>PRT</t>
-  </si>
-  <si>
     <t>GBR</t>
   </si>
   <si>
+    <t>AUT</t>
+  </si>
+  <si>
+    <t>CZE</t>
+  </si>
+  <si>
+    <t>MEX</t>
+  </si>
+  <si>
+    <t>LVA</t>
+  </si>
+  <si>
+    <t>GRC</t>
+  </si>
+  <si>
+    <t>IDN</t>
+  </si>
+  <si>
     <t>IND</t>
   </si>
   <si>
-    <t>LVA</t>
-  </si>
-  <si>
-    <t>MEX</t>
-  </si>
-  <si>
-    <t>AUT</t>
-  </si>
-  <si>
     <t>SVN</t>
   </si>
   <si>
-    <t>CZE</t>
-  </si>
-  <si>
-    <t>IDN</t>
-  </si>
-  <si>
-    <t>GRC</t>
+    <t>COL</t>
+  </si>
+  <si>
+    <t>SVK</t>
+  </si>
+  <si>
+    <t>ZAF</t>
+  </si>
+  <si>
+    <t>NLD</t>
+  </si>
+  <si>
+    <t>DEU</t>
+  </si>
+  <si>
+    <t>FRA</t>
+  </si>
+  <si>
+    <t>ITA</t>
+  </si>
+  <si>
+    <t>POL</t>
   </si>
   <si>
     <t>HUN</t>
   </si>
   <si>
-    <t>DEU</t>
-  </si>
-  <si>
-    <t>COL</t>
-  </si>
-  <si>
-    <t>SVK</t>
-  </si>
-  <si>
-    <t>ZAF</t>
-  </si>
-  <si>
-    <t>POL</t>
-  </si>
-  <si>
-    <t>NLD</t>
-  </si>
-  <si>
-    <t>ITA</t>
+    <t>JPN</t>
+  </si>
+  <si>
+    <t>BEL</t>
+  </si>
+  <si>
+    <t>CAN</t>
   </si>
   <si>
     <t>CHL</t>
   </si>
   <si>
-    <t>FRA</t>
-  </si>
-  <si>
-    <t>BEL</t>
-  </si>
-  <si>
     <t>ROU</t>
   </si>
   <si>
-    <t>JPN</t>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>NOR</t>
+  </si>
+  <si>
+    <t>BGR</t>
+  </si>
+  <si>
+    <t>LUX</t>
   </si>
   <si>
     <t>ISR</t>
   </si>
   <si>
-    <t>NOR</t>
-  </si>
-  <si>
-    <t>CAN</t>
-  </si>
-  <si>
-    <t>FIN</t>
+    <t>DNK</t>
   </si>
   <si>
     <t>RUS</t>
   </si>
   <si>
-    <t>LUX</t>
-  </si>
-  <si>
-    <t>BGR</t>
-  </si>
-  <si>
     <t>USA</t>
   </si>
   <si>
-    <t>DNK</t>
+    <t>CHE</t>
+  </si>
+  <si>
+    <t>KOR</t>
+  </si>
+  <si>
+    <t>LTU</t>
   </si>
   <si>
     <t>ARG</t>
@@ -133,28 +142,19 @@
     <t>NZL</t>
   </si>
   <si>
-    <t>CHE</t>
+    <t>SWE</t>
   </si>
   <si>
     <t>AUS</t>
   </si>
   <si>
-    <t>KOR</t>
-  </si>
-  <si>
-    <t>LTU</t>
-  </si>
-  <si>
-    <t>SWE</t>
-  </si>
-  <si>
     <t>BRA</t>
   </si>
   <si>
+    <t>TUR</t>
+  </si>
+  <si>
     <t>EST</t>
-  </si>
-  <si>
-    <t>TUR</t>
   </si>
   <si>
     <t>IRL</t>
@@ -537,7 +537,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-10.15978578256532</v>
+        <v>-10.84256769219105</v>
       </c>
       <c r="C2">
         <v>-11.19667546947339</v>
@@ -548,10 +548,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>-9.696678137128668</v>
+        <v>-9.100051706084356</v>
       </c>
       <c r="C3">
-        <v>-13.22631292791014</v>
+        <v>-10.64625044041106</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -559,10 +559,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>-8.544445269455847</v>
+        <v>-9.07591809844277</v>
       </c>
       <c r="C4">
-        <v>-10.64625044041106</v>
+        <v>-13.22631292791014</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -570,7 +570,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>-8.456685103410733</v>
+        <v>-8.564560755108985</v>
       </c>
       <c r="C5">
         <v>-9.852646439789037</v>
@@ -581,10 +581,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>-7.9973942430824</v>
+        <v>-7.990040401155996</v>
       </c>
       <c r="C6">
-        <v>-6.708090798141065</v>
+        <v>-9.638008674807697</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -592,10 +592,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>-7.752462581960118</v>
+        <v>-7.485873550599043</v>
       </c>
       <c r="C7">
-        <v>-7.332354529191843</v>
+        <v>-7.930948186647191</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -603,7 +603,7 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>-7.600996668859117</v>
+        <v>-7.430819328173033</v>
       </c>
       <c r="C8">
         <v>-6.978715886918375</v>
@@ -614,10 +614,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>-7.417233752776376</v>
+        <v>-7.417625679349705</v>
       </c>
       <c r="C9">
-        <v>-9.638008674807697</v>
+        <v>-7.332354529191843</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -625,10 +625,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>-7.142635500012984</v>
+        <v>-7.089960034675213</v>
       </c>
       <c r="C10">
-        <v>-6.866100856477953</v>
+        <v>-6.99730348543447</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -636,10 +636,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>-7.084402197959816</v>
+        <v>-7.029216690540907</v>
       </c>
       <c r="C11">
-        <v>-7.930948186647191</v>
+        <v>-7.889913754437472</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -647,10 +647,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>-7.023054791493899</v>
+        <v>-6.920758258385185</v>
       </c>
       <c r="C12">
-        <v>-7.889913754437472</v>
+        <v>-6.708090798141065</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -658,10 +658,10 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>-6.949163302323069</v>
+        <v>-6.691321462594891</v>
       </c>
       <c r="C13">
-        <v>-6.99730348543447</v>
+        <v>-6.866100856477953</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -669,10 +669,10 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>-6.465169175604634</v>
+        <v>-6.684014578593056</v>
       </c>
       <c r="C14">
-        <v>-6.094651400764151</v>
+        <v>-4.927497657010315</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -680,10 +680,10 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>-6.401301359764866</v>
+        <v>-6.602817070781553</v>
       </c>
       <c r="C15">
-        <v>-5.857047898506174</v>
+        <v>-7.108108639465415</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -691,10 +691,10 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>-6.395327831863229</v>
+        <v>-6.543400623016948</v>
       </c>
       <c r="C16">
-        <v>-4.927497657010315</v>
+        <v>-5.57904722784116</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -702,10 +702,10 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>-6.272200814254969</v>
+        <v>-6.092857805397223</v>
       </c>
       <c r="C17">
-        <v>-7.108108639465415</v>
+        <v>-5.817335417153624</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -713,10 +713,10 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>-6.212625156284435</v>
+        <v>-6.000736438855069</v>
       </c>
       <c r="C18">
-        <v>-5.57904722784116</v>
+        <v>-5.857047898506174</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -724,10 +724,10 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>-5.439909304761159</v>
+        <v>-5.837396406909379</v>
       </c>
       <c r="C19">
-        <v>-6.537818823294117</v>
+        <v>-6.195980384081645</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -735,10 +735,10 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>-5.347474700043886</v>
+        <v>-5.556722149844551</v>
       </c>
       <c r="C20">
-        <v>-5.817335417153624</v>
+        <v>-7.186499498315612</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -746,10 +746,10 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>-5.335144480318743</v>
+        <v>-5.382376865440275</v>
       </c>
       <c r="C21">
-        <v>-7.186499498315612</v>
+        <v>-6.537818823294117</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -757,10 +757,10 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>-4.790607856951201</v>
+        <v>-5.233089114857991</v>
       </c>
       <c r="C22">
-        <v>-4.371196753544937</v>
+        <v>-6.094651400764151</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -768,10 +768,10 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>-4.786250330772324</v>
+        <v>-5.151485355257057</v>
       </c>
       <c r="C23">
-        <v>-6.195980384081645</v>
+        <v>-5.039093521993943</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -779,7 +779,7 @@
         <v>25</v>
       </c>
       <c r="B24">
-        <v>-4.768342822480076</v>
+        <v>-4.748181462766976</v>
       </c>
       <c r="C24">
         <v>-4.718496431588514</v>
@@ -790,10 +790,10 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>-4.580449847085067</v>
+        <v>-4.694540393661317</v>
       </c>
       <c r="C25">
-        <v>-3.537815465093697</v>
+        <v>-3.667707077225879</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -801,10 +801,10 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <v>-4.515329443122063</v>
+        <v>-4.654475237398136</v>
       </c>
       <c r="C26">
-        <v>-5.039093521993943</v>
+        <v>-4.371196753544937</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -812,10 +812,10 @@
         <v>28</v>
       </c>
       <c r="B27">
-        <v>-4.321326240597278</v>
+        <v>-4.344019342569439</v>
       </c>
       <c r="C27">
-        <v>-5.054740417590542</v>
+        <v>-3.537815465093697</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -823,10 +823,10 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>-4.201790930837301</v>
+        <v>-4.301980120068427</v>
       </c>
       <c r="C28">
-        <v>-4.090973536006592</v>
+        <v>-3.911233965088456</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -834,10 +834,10 @@
         <v>30</v>
       </c>
       <c r="B29">
-        <v>-4.104753979113718</v>
+        <v>-4.237019737776626</v>
       </c>
       <c r="C29">
-        <v>-3.667707077225879</v>
+        <v>-4.090973536006592</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -845,10 +845,10 @@
         <v>31</v>
       </c>
       <c r="B30">
-        <v>-4.074695597547717</v>
+        <v>-4.024291911737954</v>
       </c>
       <c r="C30">
-        <v>-3.911233965088456</v>
+        <v>-5.021170765135707</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -856,10 +856,10 @@
         <v>32</v>
       </c>
       <c r="B31">
-        <v>-3.741750300047997</v>
+        <v>-4.024050416803138</v>
       </c>
       <c r="C31">
-        <v>-4.763351017441286</v>
+        <v>-0.4768904004482599</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -867,10 +867,10 @@
         <v>33</v>
       </c>
       <c r="B32">
-        <v>-3.573010644849262</v>
+        <v>-3.131566794867058</v>
       </c>
       <c r="C32">
-        <v>-0.4768904004482599</v>
+        <v>-5.054740417590542</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -878,10 +878,10 @@
         <v>34</v>
       </c>
       <c r="B33">
-        <v>-3.448813997323019</v>
+        <v>-3.066675649974193</v>
       </c>
       <c r="C33">
-        <v>-5.021170765135707</v>
+        <v>-3.072341303877146</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -889,10 +889,10 @@
         <v>35</v>
       </c>
       <c r="B34">
-        <v>-3.141538731029936</v>
+        <v>-2.987212323246624</v>
       </c>
       <c r="C34">
-        <v>-2.724829140464946</v>
+        <v>-4.763351017441286</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -900,10 +900,10 @@
         <v>36</v>
       </c>
       <c r="B35">
-        <v>-2.843829401139153</v>
+        <v>-2.978922762257352</v>
       </c>
       <c r="C35">
-        <v>-3.072341303877146</v>
+        <v>-2.724829140464946</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -911,10 +911,10 @@
         <v>37</v>
       </c>
       <c r="B36">
-        <v>-2.654062309207128</v>
+        <v>-2.866519671286338</v>
       </c>
       <c r="C36">
-        <v>-0.5149462598107779</v>
+        <v>-3.204513725473657</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -922,10 +922,10 @@
         <v>38</v>
       </c>
       <c r="B37">
-        <v>-2.203228322798689</v>
+        <v>-2.809799064301033</v>
       </c>
       <c r="C37">
-        <v>-2.394044212023194</v>
+        <v>-1.520234890225636</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -933,10 +933,10 @@
         <v>39</v>
       </c>
       <c r="B38">
-        <v>-2.186168475262518</v>
+        <v>-2.233135578402801</v>
       </c>
       <c r="C38">
-        <v>-3.204513725473657</v>
+        <v>-1.065470275273439</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -944,10 +944,10 @@
         <v>40</v>
       </c>
       <c r="B39">
-        <v>-2.108799170480524</v>
+        <v>-2.20202653678967</v>
       </c>
       <c r="C39">
-        <v>-1.926032824459722</v>
+        <v>-0.5149462598107779</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -955,10 +955,10 @@
         <v>41</v>
       </c>
       <c r="B40">
-        <v>-1.991830234587555</v>
+        <v>-1.914077508116385</v>
       </c>
       <c r="C40">
-        <v>-1.520234890225636</v>
+        <v>-2.394044212023194</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -966,10 +966,10 @@
         <v>42</v>
       </c>
       <c r="B41">
-        <v>-1.799167037248128</v>
+        <v>-1.655265079906953</v>
       </c>
       <c r="C41">
-        <v>-1.065470275273439</v>
+        <v>-2.362646798756485</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -977,10 +977,10 @@
         <v>43</v>
       </c>
       <c r="B42">
-        <v>-1.716066991605669</v>
+        <v>-1.637548339092287</v>
       </c>
       <c r="C42">
-        <v>-2.362646798756485</v>
+        <v>-1.926032824459722</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -988,7 +988,7 @@
         <v>44</v>
       </c>
       <c r="B43">
-        <v>-1.411667235809122</v>
+        <v>-1.161355094468497</v>
       </c>
       <c r="C43">
         <v>-2.555628819729538</v>
@@ -999,10 +999,10 @@
         <v>45</v>
       </c>
       <c r="B44">
-        <v>1.626755667568891</v>
+        <v>1.506455358114889</v>
       </c>
       <c r="C44">
-        <v>0.80954414990968</v>
+        <v>4.746288661325582</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1010,10 +1010,10 @@
         <v>46</v>
       </c>
       <c r="B45">
-        <v>2.195022431022609</v>
+        <v>3.06213806776201</v>
       </c>
       <c r="C45">
-        <v>4.746288661325582</v>
+        <v>0.80954414990968</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1021,7 +1021,7 @@
         <v>47</v>
       </c>
       <c r="B46">
-        <v>5.320998101305019</v>
+        <v>4.404226135719469</v>
       </c>
       <c r="C46">
         <v>10.1997158035124</v>

</xml_diff>